<commit_message>
all of workers tasks
</commit_message>
<xml_diff>
--- a/pm.v3.xlsx
+++ b/pm.v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="11232" windowHeight="2304" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="11232" windowHeight="2304" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -3143,8 +3143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="76" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3285,7 +3285,7 @@
     <row r="13" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="6"/>

</xml_diff>

<commit_message>
lil ch worker x2
</commit_message>
<xml_diff>
--- a/pm.v3.xlsx
+++ b/pm.v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="11232" windowHeight="2304" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="11232" windowHeight="2304" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Админ</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>o  Управление задачами: создание, назначение исполнителей</t>
+  </si>
+  <si>
+    <t>селект(год/месяц/неделя)</t>
+  </si>
+  <si>
+    <t>селект (исполнитель/проект)</t>
+  </si>
+  <si>
+    <t>(+)</t>
   </si>
 </sst>
 </file>
@@ -3141,10 +3150,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="76" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="76" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3154,7 +3163,7 @@
     <col min="4" max="4" width="47.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3166,7 +3175,7 @@
       </c>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>11</v>
       </c>
@@ -3176,7 +3185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
@@ -3186,7 +3195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>13</v>
       </c>
@@ -3194,7 +3203,7 @@
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>14</v>
       </c>
@@ -3208,7 +3217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="32" t="s">
         <v>41</v>
@@ -3220,7 +3229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="25" t="s">
         <v>18</v>
@@ -3232,7 +3241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="32" t="s">
         <v>20</v>
@@ -3242,7 +3251,7 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="22" t="s">
         <v>22</v>
@@ -3252,7 +3261,7 @@
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="32" t="s">
         <v>24</v>
@@ -3264,7 +3273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="10"/>
       <c r="C11" s="23" t="s">
@@ -3274,23 +3283,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="10"/>
       <c r="C12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="10"/>
       <c r="C13" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -3300,7 +3318,7 @@
       <c r="C14" s="11"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>28</v>
       </c>
@@ -3310,7 +3328,7 @@
       <c r="C15" s="11"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>30</v>
       </c>

</xml_diff>